<commit_message>
Last Sync: 2026-01-17 13:41 (Mobile)
</commit_message>
<xml_diff>
--- a/Recruitment/Jan 2026.xlsx
+++ b/Recruitment/Jan 2026.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkumar10\Downloads\SVJK_Telecalling_Status\Recruitment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D701AAD-B71C-4986-A28D-95977352B7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{1E5C3204-E011-ED48-9B00-BE35C1F0C56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>Recruitment Telecalling Leads</t>
   </si>
@@ -75,6 +88,9 @@
   </si>
   <si>
     <t>Aishwarya Koppal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -502,18 +518,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.48046875" customWidth="1"/>
+    <col min="2" max="3" width="19.7734375" customWidth="1"/>
+    <col min="4" max="4" width="44.390625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -521,7 +537,7 @@
       <c r="C1" s="12"/>
       <c r="D1" s="13"/>
     </row>
-    <row r="2" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -535,7 +551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -549,7 +565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -563,7 +579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -577,7 +593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -591,7 +607,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
@@ -605,7 +621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -619,7 +635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -633,7 +649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
@@ -647,7 +663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -661,7 +677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
@@ -675,127 +691,129 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -812,6 +830,6 @@
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{d5b0e46e-af26-40f8-bc06-c0e471e18c78}" enabled="1" method="Privileged" siteId="{9bc3d1cd-55ca-4e13-b5a2-a9e9deaeba3f}" contentBits="0" removed="0"/>
+  <clbl:label id="{d5b0e46e-af26-40f8-bc06-c0e471e18c78}" enabled="1" method="Privileged" siteId="{9bc3d1cd-55ca-4e13-b5a2-a9e9deaeba3f}" contentBits="4" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>